<commit_message>
vault backup: 2026-02-03 21:19:04
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17655"/>
+    <workbookView windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="132">
   <si>
     <t>Products/solutions provided</t>
   </si>
@@ -1323,49 +1323,50 @@
     <t>EDF Energy (UK)</t>
   </si>
   <si>
-    <t>UK arm of EDF Group</t>
+    <t>€118,690 million</t>
+  </si>
+  <si>
+    <t>France, UK, Italy, Belgium</t>
+  </si>
+  <si>
+    <t>Large UK network</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>EV tariff “GoElectric”</t>
+  </si>
+  <si>
+    <t>Usage EV tariffs</t>
+  </si>
+  <si>
+    <t>No known V2G</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Correction: Your PDF screenshot (Page 2, "Sales") explicitly states 118,690 for 2024.
+URL: https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf</t>
+  </si>
+  <si>
+    <t>EV tariff exists.</t>
+  </si>
+  <si>
+    <t>V2G not in mainstream tariff info</t>
+  </si>
+  <si>
+    <t>SottishPower</t>
+  </si>
+  <si>
+    <t>SSE plc (UK)</t>
+  </si>
+  <si>
+    <t>Major UK supplier</t>
   </si>
   <si>
     <t>UK</t>
-  </si>
-  <si>
-    <t>Large UK network</t>
-  </si>
-  <si>
-    <t>—</t>
-  </si>
-  <si>
-    <t>EV tariff “GoElectric”</t>
-  </si>
-  <si>
-    <t>Usage EV tariffs</t>
-  </si>
-  <si>
-    <t>No known V2G</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>UK “GoElectric Overnight” EV tariff. (ev.energy)</t>
-  </si>
-  <si>
-    <t>测试</t>
-  </si>
-  <si>
-    <t>EV tariff exists.</t>
-  </si>
-  <si>
-    <t>V2G not in mainstream tariff info</t>
-  </si>
-  <si>
-    <t>SottishPower</t>
-  </si>
-  <si>
-    <t>SSE plc (UK)</t>
-  </si>
-  <si>
-    <t>Major UK supplier</t>
   </si>
   <si>
     <t>Millions</t>
@@ -1522,7 +1523,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1554,6 +1555,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2035,150 +2044,150 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2198,12 +2207,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2534,8 +2546,8 @@
   <sheetPr/>
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>
@@ -2557,11 +2569,11 @@
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="4" t="s">
@@ -2594,7 +2606,7 @@
       <c r="J2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -2635,7 +2647,7 @@
       <c r="H3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="13" t="s">
         <v>26</v>
       </c>
       <c r="J3" s="7" t="s">
@@ -2761,7 +2773,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="10" t="s">
         <v>65</v>
       </c>
       <c r="G6" s="6"/>
@@ -2825,16 +2837,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" ht="28.5" spans="1:15">
+    <row r="8" ht="128.25" spans="1:15">
       <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>78</v>
-      </c>
+      <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2842,10 +2852,10 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -2854,7 +2864,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2873,13 +2883,13 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>84</v>
@@ -2969,10 +2979,10 @@
       <c r="A12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>97</v>
       </c>
       <c r="D12" s="6"/>
@@ -3039,7 +3049,7 @@
       <c r="A14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>105</v>
       </c>
       <c r="C14" s="6"/>
@@ -3107,7 +3117,7 @@
       <c r="A16" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="10" t="s">
         <v>114</v>
       </c>
       <c r="C16" s="6"/>
@@ -3175,7 +3185,7 @@
       <c r="A18" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C18" s="6"/>
@@ -3243,7 +3253,7 @@
       <c r="A20" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>131</v>
       </c>
       <c r="C20" s="6"/>
@@ -3269,13 +3279,13 @@
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" display="E.ON Next Drive offers EV‑oriented tariff. (ev.energy)"/>
     <hyperlink ref="F6" r:id="rId2" display="E.ON Next offers Time‑of‑Use Smart Saver tariff. (太阳报)"/>
-    <hyperlink ref="B8" r:id="rId1" display="UK “GoElectric Overnight” EV tariff. (ev.energy)"/>
-    <hyperlink ref="B12" r:id="rId3" display="Statkraft is Europe’s largest renewable energy producer. (维基百科)"/>
-    <hyperlink ref="C12" r:id="rId4" display="Operates EV charging solutions via Mer across multiple European markets. (Mer)"/>
-    <hyperlink ref="B14" r:id="rId5" display="Vattenfall operates one of Europe’s larger EV networks (InCharge). (Vattenfall)"/>
-    <hyperlink ref="B16" r:id="rId6" display="Equinor primarily oil/energy with expanding renewables. (维基百科)"/>
-    <hyperlink ref="B18" r:id="rId7" display="Major utility with renewables &amp; EV charging expansion in Spain/Portugal. (维基百科)"/>
-    <hyperlink ref="B20" r:id="rId8" display="Poland’s largest utility; BESS project planned; India involvement. (维基百科)"/>
+    <hyperlink ref="B8" r:id="rId3" display="Correction: Your PDF screenshot (Page 2, &quot;Sales&quot;) explicitly states 118,690 for 2024.&#10;URL: https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf" tooltip="https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf"/>
+    <hyperlink ref="B12" r:id="rId4" display="Statkraft is Europe’s largest renewable energy producer. (维基百科)"/>
+    <hyperlink ref="C12" r:id="rId5" display="Operates EV charging solutions via Mer across multiple European markets. (Mer)"/>
+    <hyperlink ref="B14" r:id="rId6" display="Vattenfall operates one of Europe’s larger EV networks (InCharge). (Vattenfall)"/>
+    <hyperlink ref="B16" r:id="rId7" display="Equinor primarily oil/energy with expanding renewables. (维基百科)"/>
+    <hyperlink ref="B18" r:id="rId8" display="Major utility with renewables &amp; EV charging expansion in Spain/Portugal. (维基百科)"/>
+    <hyperlink ref="B20" r:id="rId9" display="Poland’s largest utility; BESS project planned; India involvement. (维基百科)"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
vault backup: 2026-02-03 21:31:42
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="133">
   <si>
     <t>Products/solutions provided</t>
   </si>
@@ -1326,7 +1326,7 @@
     <t>€118,690 million</t>
   </si>
   <si>
-    <t>France, UK, Italy, Belgium</t>
+    <t>France, United Kingdom, Italy</t>
   </si>
   <si>
     <t>Large UK network</t>
@@ -1347,8 +1347,12 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Correction: Your PDF screenshot (Page 2, "Sales") explicitly states 118,690 for 2024.
+    <t>Correction: The PDF screenshot (Page 2, "Sales") explicitly states 118,690 for 2024.
 URL: https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf</t>
+  </si>
+  <si>
+    <t>Source: Page 32, Note 5.2 text (mentions principal segments: France, UK, Italy).
+https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf</t>
   </si>
   <si>
     <t>EV tariff exists.</t>
@@ -2187,7 +2191,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2211,6 +2215,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2547,7 +2554,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>
@@ -2569,11 +2576,11 @@
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="4" t="s">
@@ -2606,7 +2613,7 @@
       <c r="J2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="13" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -2647,7 +2654,7 @@
       <c r="H3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="14" t="s">
         <v>26</v>
       </c>
       <c r="J3" s="7" t="s">
@@ -2837,14 +2844,16 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" ht="128.25" spans="1:15">
+    <row r="8" ht="114" spans="1:15">
       <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="11" t="s">
+        <v>78</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2852,10 +2861,10 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -2864,7 +2873,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2883,16 +2892,16 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>72</v>
@@ -2910,10 +2919,10 @@
         <v>72</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>72</v>
@@ -2930,28 +2939,28 @@
     </row>
     <row r="11" ht="28.5" spans="1:15">
       <c r="A11" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>72</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>72</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>72</v>
@@ -2966,13 +2975,13 @@
         <v>72</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" ht="42.75" spans="1:15">
@@ -2980,10 +2989,10 @@
         <v>63</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -3000,28 +3009,28 @@
     </row>
     <row r="13" ht="15" spans="1:15">
       <c r="A13" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>72</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>72</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>72</v>
@@ -3039,10 +3048,10 @@
         <v>76</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" ht="42.75" spans="1:15">
@@ -3050,7 +3059,7 @@
         <v>63</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -3068,16 +3077,16 @@
     </row>
     <row r="15" ht="28.5" spans="1:15">
       <c r="A15" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>72</v>
@@ -3089,7 +3098,7 @@
         <v>72</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>72</v>
@@ -3104,13 +3113,13 @@
         <v>72</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" ht="42.75" spans="1:15">
@@ -3118,7 +3127,7 @@
         <v>63</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -3136,28 +3145,28 @@
     </row>
     <row r="17" ht="28.5" spans="1:15">
       <c r="A17" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>72</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>72</v>
@@ -3166,7 +3175,7 @@
         <v>72</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>72</v>
@@ -3186,7 +3195,7 @@
         <v>63</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -3204,28 +3213,28 @@
     </row>
     <row r="19" ht="28.5" spans="1:15">
       <c r="A19" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>72</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>72</v>
@@ -3254,7 +3263,7 @@
         <v>63</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -3279,13 +3288,14 @@
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" display="E.ON Next Drive offers EV‑oriented tariff. (ev.energy)"/>
     <hyperlink ref="F6" r:id="rId2" display="E.ON Next offers Time‑of‑Use Smart Saver tariff. (太阳报)"/>
-    <hyperlink ref="B8" r:id="rId3" display="Correction: Your PDF screenshot (Page 2, &quot;Sales&quot;) explicitly states 118,690 for 2024.&#10;URL: https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf" tooltip="https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf"/>
+    <hyperlink ref="B8" r:id="rId3" display="Correction: The PDF screenshot (Page 2, &quot;Sales&quot;) explicitly states 118,690 for 2024.&#10;URL: https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf" tooltip="https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf"/>
     <hyperlink ref="B12" r:id="rId4" display="Statkraft is Europe’s largest renewable energy producer. (维基百科)"/>
     <hyperlink ref="C12" r:id="rId5" display="Operates EV charging solutions via Mer across multiple European markets. (Mer)"/>
     <hyperlink ref="B14" r:id="rId6" display="Vattenfall operates one of Europe’s larger EV networks (InCharge). (Vattenfall)"/>
     <hyperlink ref="B16" r:id="rId7" display="Equinor primarily oil/energy with expanding renewables. (维基百科)"/>
     <hyperlink ref="B18" r:id="rId8" display="Major utility with renewables &amp; EV charging expansion in Spain/Portugal. (维基百科)"/>
     <hyperlink ref="B20" r:id="rId9" display="Poland’s largest utility; BESS project planned; India involvement. (维基百科)"/>
+    <hyperlink ref="C8" r:id="rId3" display="Source: Page 32, Note 5.2 text (mentions principal segments: France, UK, Italy).&#10;https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
vault backup: 2026-02-03 21:59:09
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="134">
   <si>
     <t>Products/solutions provided</t>
   </si>
@@ -1329,7 +1329,8 @@
     <t>France, United Kingdom, Italy</t>
   </si>
   <si>
-    <t>Large UK network</t>
+    <t>Global: 41.5 Million;
+UK: ~3.7 Million (Est.)</t>
   </si>
   <si>
     <t>—</t>
@@ -1353,6 +1354,11 @@
   <si>
     <t>Source: Page 32, Note 5.2 text (mentions principal segments: France, UK, Italy).
 https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf</t>
+  </si>
+  <si>
+    <t>Source: Global: Page 3 ("residential customer portfolio... 41.5 million").
+Note: UK figure not separately disclosed in 2024 text; value is estimated based on 2023 figures.
+https://www.edf.fr/sites/groupe/files/2025-02/edf-annual-results-2024-management-report-2025-02-21.pdf</t>
   </si>
   <si>
     <t>EV tariff exists.</t>
@@ -2554,7 +2560,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>
@@ -2797,7 +2803,7 @@
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" ht="28.5" spans="1:15">
       <c r="A7" s="5" t="s">
         <v>68</v>
       </c>
@@ -2844,7 +2850,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" ht="114" spans="1:15">
+    <row r="8" ht="156.75" spans="1:15">
       <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
@@ -2854,17 +2860,19 @@
       <c r="C8" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -2873,7 +2881,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2892,16 +2900,16 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>72</v>
@@ -2919,10 +2927,10 @@
         <v>72</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>72</v>
@@ -2939,28 +2947,28 @@
     </row>
     <row r="11" ht="28.5" spans="1:15">
       <c r="A11" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>72</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>72</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>72</v>
@@ -2975,13 +2983,13 @@
         <v>72</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" ht="42.75" spans="1:15">
@@ -2989,10 +2997,10 @@
         <v>63</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -3009,28 +3017,28 @@
     </row>
     <row r="13" ht="15" spans="1:15">
       <c r="A13" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>72</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>72</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>72</v>
@@ -3048,10 +3056,10 @@
         <v>76</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" ht="42.75" spans="1:15">
@@ -3059,7 +3067,7 @@
         <v>63</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -3077,16 +3085,16 @@
     </row>
     <row r="15" ht="28.5" spans="1:15">
       <c r="A15" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>72</v>
@@ -3098,7 +3106,7 @@
         <v>72</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>72</v>
@@ -3113,13 +3121,13 @@
         <v>72</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" ht="42.75" spans="1:15">
@@ -3127,7 +3135,7 @@
         <v>63</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -3145,28 +3153,28 @@
     </row>
     <row r="17" ht="28.5" spans="1:15">
       <c r="A17" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>72</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>72</v>
@@ -3175,7 +3183,7 @@
         <v>72</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>72</v>
@@ -3195,7 +3203,7 @@
         <v>63</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -3213,28 +3221,28 @@
     </row>
     <row r="19" ht="28.5" spans="1:15">
       <c r="A19" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>72</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>72</v>
@@ -3263,7 +3271,7 @@
         <v>63</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>

</xml_diff>

<commit_message>
vault backup: 2026-02-03 22:10:49
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="139">
   <si>
     <t>Products/solutions provided</t>
   </si>
@@ -1323,17 +1323,115 @@
     <t>EDF Energy (UK)</t>
   </si>
   <si>
-    <t>€118,690 million</t>
-  </si>
-  <si>
-    <t>France, United Kingdom, Italy</t>
-  </si>
-  <si>
-    <t>Global: 41.5 Million;
-UK: ~3.7 Million (Est.)</t>
-  </si>
-  <si>
-    <t>—</t>
+    <r>
+      <t>€118.7 Billion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (Group Sales 2024);
+UK Segment Revenue: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>~€13.6 Billion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (Est.).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">France (HQ), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>UK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>, Italy (Edison), Belgium (Luminus);
+Active in 20+ countries worldwide.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">41.5 Million </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>customer sites globally;
+~</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3.7 Million</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> in the UK (Residential &amp; Business).</t>
+    </r>
+  </si>
+  <si>
+    <t>Partnership with DriveElectric (Personal &amp; Business leasing); Offers varying makes (Tesla, MG, Nissan, etc.).</t>
+  </si>
+  <si>
+    <t>Home: Pod Point Solo 3 (7kW, tethered/untethered).
+Public: Pod Point Network (Tesco partnership, Lidl, etc.).</t>
+  </si>
+  <si>
+    <t>Powervault 3 (Eco-Store partnership); Also installs Tesla Powerwall 2 and Sonnen via partners.</t>
+  </si>
+  <si>
+    <t>Installer: EDF Renewables / Hometech.
+Hardware: Tier 1 Panels (e.g., Sharp, JA Solar); Inverters: Solis or Growatt.</t>
+  </si>
+  <si>
+    <t>Partnership with CB Heating (EDF acquired them).
+Hardware: Primarily Daikin (Altherma 3) and Mitsubishi Electric (Ecodan).</t>
   </si>
   <si>
     <t>EV tariff “GoElectric”</t>
@@ -1380,6 +1478,9 @@
   </si>
   <si>
     <t>Millions</t>
+  </si>
+  <si>
+    <t>—</t>
   </si>
   <si>
     <t>Standard &amp; evolving TOU</t>
@@ -2560,7 +2661,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>
@@ -2803,51 +2904,51 @@
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
     </row>
-    <row r="7" ht="28.5" spans="1:15">
+    <row r="7" ht="71.25" spans="1:15">
       <c r="A7" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>71</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>72</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" ht="156.75" spans="1:15">
@@ -2855,13 +2956,13 @@
         <v>63</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2869,10 +2970,10 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -2881,7 +2982,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2900,96 +3001,96 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" ht="28.5" spans="1:15">
       <c r="A11" s="5" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>72</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" ht="42.75" spans="1:15">
@@ -2997,10 +3098,10 @@
         <v>63</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -3017,49 +3118,49 @@
     </row>
     <row r="13" ht="15" spans="1:15">
       <c r="A13" s="5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" ht="42.75" spans="1:15">
@@ -3067,7 +3168,7 @@
         <v>63</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -3085,49 +3186,49 @@
     </row>
     <row r="15" ht="28.5" spans="1:15">
       <c r="A15" s="5" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" ht="42.75" spans="1:15">
@@ -3135,7 +3236,7 @@
         <v>63</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -3153,49 +3254,49 @@
     </row>
     <row r="17" ht="28.5" spans="1:15">
       <c r="A17" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" ht="42.75" spans="1:15">
@@ -3203,7 +3304,7 @@
         <v>63</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -3221,49 +3322,49 @@
     </row>
     <row r="19" ht="28.5" spans="1:15">
       <c r="A19" s="5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" ht="42.75" spans="1:15">
@@ -3271,7 +3372,7 @@
         <v>63</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>

</xml_diff>

<commit_message>
vault backup: 2026-02-03 22:23:00
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="140">
   <si>
     <t>Products/solutions provided</t>
   </si>
@@ -1416,7 +1416,28 @@
     </r>
   </si>
   <si>
-    <t>Partnership with DriveElectric (Personal &amp; Business leasing); Offers varying makes (Tesla, MG, Nissan, etc.).</t>
+    <r>
+      <t xml:space="preserve">Partnership with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>DriveElectric</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (Personal &amp; Business); offers integrated "Full Solution" bundle (Car + Pod Point Charger + Tariff).</t>
+    </r>
   </si>
   <si>
     <t>Home: Pod Point Solo 3 (7kW, tethered/untethered).
@@ -1457,6 +1478,9 @@
     <t>Source: Global: Page 3 ("residential customer portfolio... 41.5 million").
 Note: UK figure not separately disclosed in 2024 text; value is estimated based on 2023 figures.
 https://www.edf.fr/sites/groupe/files/2025-02/edf-annual-results-2024-management-report-2025-02-21.pdf</t>
+  </si>
+  <si>
+    <t>https://www.edfenergy.com/electric-cars/leasing</t>
   </si>
   <si>
     <t>EV tariff exists.</t>
@@ -2298,7 +2322,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2325,6 +2349,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2660,8 +2687,8 @@
   <sheetPr/>
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>
@@ -2683,11 +2710,11 @@
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="4" t="s">
@@ -2720,7 +2747,7 @@
       <c r="J2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="14" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -2761,7 +2788,7 @@
       <c r="H3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="15" t="s">
         <v>26</v>
       </c>
       <c r="J3" s="7" t="s">
@@ -2961,19 +2988,21 @@
       <c r="C8" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -2982,7 +3011,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -3001,40 +3030,40 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J10" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>80</v>
@@ -3048,49 +3077,49 @@
     </row>
     <row r="11" ht="28.5" spans="1:15">
       <c r="A11" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" ht="42.75" spans="1:15">
@@ -3098,10 +3127,10 @@
         <v>63</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -3118,49 +3147,49 @@
     </row>
     <row r="13" ht="15" spans="1:15">
       <c r="A13" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M13" s="6" t="s">
         <v>80</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" ht="42.75" spans="1:15">
@@ -3168,7 +3197,7 @@
         <v>63</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -3186,49 +3215,49 @@
     </row>
     <row r="15" ht="28.5" spans="1:15">
       <c r="A15" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" ht="42.75" spans="1:15">
@@ -3236,7 +3265,7 @@
         <v>63</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -3254,40 +3283,40 @@
     </row>
     <row r="17" ht="28.5" spans="1:15">
       <c r="A17" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>80</v>
@@ -3304,7 +3333,7 @@
         <v>63</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -3322,40 +3351,40 @@
     </row>
     <row r="19" ht="28.5" spans="1:15">
       <c r="A19" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M19" s="6" t="s">
         <v>80</v>
@@ -3372,7 +3401,7 @@
         <v>63</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -3405,6 +3434,8 @@
     <hyperlink ref="B18" r:id="rId8" display="Major utility with renewables &amp; EV charging expansion in Spain/Portugal. (维基百科)"/>
     <hyperlink ref="B20" r:id="rId9" display="Poland’s largest utility; BESS project planned; India involvement. (维基百科)"/>
     <hyperlink ref="C8" r:id="rId3" display="Source: Page 32, Note 5.2 text (mentions principal segments: France, UK, Italy).&#10;https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf"/>
+    <hyperlink ref="E8" r:id="rId10" display="https://www.edfenergy.com/electric-cars/leasing" tooltip="https://www.edfenergy.com/electric-cars/leasing"/>
+    <hyperlink ref="D8" r:id="rId11" display="Source: Global: Page 3 (&quot;residential customer portfolio... 41.5 million&quot;).&#10;Note: UK figure not separately disclosed in 2024 text; value is estimated based on 2023 figures.&#10;https://www.edf.fr/sites/groupe/files/2025-02/edf-annual-results-2024-management-report-2025-02-21.pdf"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
vault backup: 2026-02-03 22:49:40
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="143">
   <si>
     <t>Products/solutions provided</t>
   </si>
@@ -1440,15 +1440,18 @@
     </r>
   </si>
   <si>
-    <t>Home: Pod Point Solo 3 (7kW, tethered/untethered).
-Public: Pod Point Network (Tesco partnership, Lidl, etc.).</t>
-  </si>
-  <si>
-    <t>Powervault 3 (Eco-Store partnership); Also installs Tesla Powerwall 2 and Sonnen via partners.</t>
-  </si>
-  <si>
-    <t>Installer: EDF Renewables / Hometech.
-Hardware: Tier 1 Panels (e.g., Sharp, JA Solar); Inverters: Solis or Growatt.</t>
+    <t>Home: Pod Point Solo 3S (7kW, Solar integrated).
+Offers: 1. Upfront purchase; 2. "Plug &amp; Power" bundle (Hardware discount with Tariff); 3. "Pod Drive" (0 upfront, monthly subscription).
+Public: Pod Point Network (Strategic partner; Tesco/Lidl locations).</t>
+  </si>
+  <si>
+    <t>Installer: Contact Solar.
+Hardware: Flexible Tier 1 Modular Systems.
+Note: No specific brand advertised (e.g., no Tesla/Powervault). Focus on cost-effective, mid-range solutions.</t>
+  </si>
+  <si>
+    <t>Installer: Contact Solar (EDF Owned).
+Hardware: Standard Tier 1 Monocrystalline (White-label strategy, brands vary by stock).</t>
   </si>
   <si>
     <t>Partnership with CB Heating (EDF acquired them).
@@ -1481,6 +1484,18 @@
   </si>
   <si>
     <t>https://www.edfenergy.com/electric-cars/leasing</t>
+  </si>
+  <si>
+    <t>https://www.edfenergy.com/electric-cars/home-charger</t>
+  </si>
+  <si>
+    <t>Adopts a "Hardware Agnostic" strategy: No premium brands (like Tesla Powerwall) are advertised. Focuses on modular, cost-effective solutions installed in-house to maximize margins.
+Link: https://www.contact-solar.co.uk/battery-storage/</t>
+  </si>
+  <si>
+    <t>Fulfilled by EDF's subsidiary "Contact Solar". Marketing emphasizes technology types (String vs. Micro inverters) rather than specific manufacturers, allowing for flexible Tier 1 hardware sourcing.
+Link: 
+https://www.contact-solar.co.uk/help-center/our-panels-inverters/</t>
   </si>
   <si>
     <t>EV tariff exists.</t>
@@ -2687,8 +2702,10 @@
   <sheetPr/>
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>
@@ -2931,7 +2948,7 @@
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
     </row>
-    <row r="7" ht="71.25" spans="1:15">
+    <row r="7" ht="142.5" spans="1:15">
       <c r="A7" s="5" t="s">
         <v>68</v>
       </c>
@@ -2978,7 +2995,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" ht="156.75" spans="1:15">
+    <row r="8" ht="171" spans="1:15">
       <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
@@ -2994,15 +3011,21 @@
       <c r="E8" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="F8" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -3011,7 +3034,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -3030,40 +3053,40 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>80</v>
@@ -3077,49 +3100,49 @@
     </row>
     <row r="11" ht="28.5" spans="1:15">
       <c r="A11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>92</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" ht="42.75" spans="1:15">
@@ -3127,10 +3150,10 @@
         <v>63</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -3147,49 +3170,49 @@
     </row>
     <row r="13" ht="15" spans="1:15">
       <c r="A13" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="M13" s="6" t="s">
         <v>80</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" ht="42.75" spans="1:15">
@@ -3197,7 +3220,7 @@
         <v>63</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -3215,49 +3238,49 @@
     </row>
     <row r="15" ht="28.5" spans="1:15">
       <c r="A15" s="5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" ht="42.75" spans="1:15">
@@ -3265,7 +3288,7 @@
         <v>63</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -3283,40 +3306,40 @@
     </row>
     <row r="17" ht="28.5" spans="1:15">
       <c r="A17" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>80</v>
@@ -3333,7 +3356,7 @@
         <v>63</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -3351,40 +3374,40 @@
     </row>
     <row r="19" ht="28.5" spans="1:15">
       <c r="A19" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="M19" s="6" t="s">
         <v>80</v>
@@ -3401,7 +3424,7 @@
         <v>63</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -3436,6 +3459,8 @@
     <hyperlink ref="C8" r:id="rId3" display="Source: Page 32, Note 5.2 text (mentions principal segments: France, UK, Italy).&#10;https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf"/>
     <hyperlink ref="E8" r:id="rId10" display="https://www.edfenergy.com/electric-cars/leasing" tooltip="https://www.edfenergy.com/electric-cars/leasing"/>
     <hyperlink ref="D8" r:id="rId11" display="Source: Global: Page 3 (&quot;residential customer portfolio... 41.5 million&quot;).&#10;Note: UK figure not separately disclosed in 2024 text; value is estimated based on 2023 figures.&#10;https://www.edf.fr/sites/groupe/files/2025-02/edf-annual-results-2024-management-report-2025-02-21.pdf"/>
+    <hyperlink ref="F8" r:id="rId12" display="https://www.edfenergy.com/electric-cars/home-charger"/>
+    <hyperlink ref="H8" r:id="rId13" display="Fulfilled by EDF's subsidiary &quot;Contact Solar&quot;. Marketing emphasizes technology types (String vs. Micro inverters) rather than specific manufacturers, allowing for flexible Tier 1 hardware sourcing.&#10;Link: &#10;https://www.contact-solar.co.uk/help-center/our-panels-inverters/" tooltip="https://www.contact-solar.co.uk/help-center/our-panels-inverters/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
vault backup: 2026-02-03 23:37:05
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="150">
   <si>
     <t>Products/solutions provided</t>
   </si>
@@ -1454,20 +1454,26 @@
 Hardware: Standard Tier 1 Monocrystalline (White-label strategy, brands vary by stock).</t>
   </si>
   <si>
-    <t>Partnership with CB Heating (EDF acquired them).
-Hardware: Primarily Daikin (Altherma 3) and Mitsubishi Electric (Ecodan).</t>
-  </si>
-  <si>
-    <t>EV tariff “GoElectric”</t>
-  </si>
-  <si>
-    <t>Usage EV tariffs</t>
-  </si>
-  <si>
-    <t>No known V2G</t>
-  </si>
-  <si>
-    <t>Yes</t>
+    <t>Partner: CB Heating
+(Hardware: Daikin, Ideal)</t>
+  </si>
+  <si>
+    <t>GoElectric Overnight (Fixed 5-hour off-peak window: 12am-5am). Requires Smart Meter; Designed for EV drivers to lock in lower overnight charging rates.</t>
+  </si>
+  <si>
+    <t>Heat Pump Tracker (Exclusive to EDF Heat Pump customers); Offers daily savings &amp; "Zero Carbon" electricity guarantee. Bundled with installation service.</t>
+  </si>
+  <si>
+    <t>Commercial/Fleet focus only. No public "Domestic" V2G tier yet; prioritizes "Smart Charging" (V1G) via Pod Point for residential users rather than bi-directional discharge.</t>
+  </si>
+  <si>
+    <t>Market Leader (Big 6 Supplier). "Britain's biggest generator of zero carbon electricity". Focus on heat pumps &amp; solar integration.</t>
+  </si>
+  <si>
+    <t>Comprehensive Workplace &amp; Fleet solutions via subsidiary "Pod Point". Offers "Commercial Charging" for businesses.</t>
+  </si>
+  <si>
+    <t>Operates one of the UK's largest "Destination Charging" networks. Strategy focuses on retail locations (e.g., exclusive rollout for Tesco and Lidl) rather than motorway rapid hubs.</t>
   </si>
   <si>
     <t>Correction: The PDF screenshot (Page 2, "Sales") explicitly states 118,690 for 2024.
@@ -1490,7 +1496,8 @@
   </si>
   <si>
     <t>Adopts a "Hardware Agnostic" strategy: No premium brands (like Tesla Powerwall) are advertised. Focuses on modular, cost-effective solutions installed in-house to maximize margins.
-Link: https://www.contact-solar.co.uk/battery-storage/</t>
+Link: 
+https://www.contact-solar.co.uk/battery-storage/</t>
   </si>
   <si>
     <t>Fulfilled by EDF's subsidiary "Contact Solar". Marketing emphasizes technology types (String vs. Micro inverters) rather than specific manufacturers, allowing for flexible Tier 1 hardware sourcing.
@@ -1498,10 +1505,30 @@
 https://www.contact-solar.co.uk/help-center/our-panels-inverters/</t>
   </si>
   <si>
-    <t>EV tariff exists.</t>
-  </si>
-  <si>
-    <t>V2G not in mainstream tariff info</t>
+    <t>Source: https://www.cbheating.co.uk/
+Footer: "CB Heating Ltd trading as EDF Heat Pumps"</t>
+  </si>
+  <si>
+    <t>Source: https://www.edfenergy.com/electric-cars/ev-tariffs
+Screenshot 2: "Five hours... 12am-5am"</t>
+  </si>
+  <si>
+    <t>Source: https://www.edfenergy.com/heating
+Screenshot 2 (Checklist): "Heat pump tariffs"</t>
+  </si>
+  <si>
+    <t>Source: https://www.edfenergy.com/electric-cars/charging-points
+Screenshot 4: Title "Workplace EV charging"</t>
+  </si>
+  <si>
+    <t>Source: EDF Official Site (Homepage)
+Link: https://www.edfenergy.com/
+Quote: "Britain's biggest generator of zero carbon electricity."</t>
+  </si>
+  <si>
+    <t>Source: Pod Point Homepage (EDF Group)
+Link: https://pod-point.com/
+Quote: Top Menu Bar: "Commercial charging" / "Workplace"</t>
   </si>
   <si>
     <t>SottishPower</t>
@@ -1526,6 +1553,9 @@
   </si>
   <si>
     <t>Standard segments</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
   <si>
     <t>Statkraft (via Mer)</t>
@@ -2702,10 +2732,10 @@
   <sheetPr/>
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>
@@ -2989,10 +3019,10 @@
         <v>80</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" ht="171" spans="1:15">
@@ -3000,41 +3030,49 @@
         <v>63</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I8" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="J8" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+        <v>92</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -3053,96 +3091,96 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" ht="28.5" spans="1:15">
       <c r="A11" s="5" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>95</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" ht="42.75" spans="1:15">
@@ -3150,10 +3188,10 @@
         <v>63</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -3170,49 +3208,49 @@
     </row>
     <row r="13" ht="15" spans="1:15">
       <c r="A13" s="5" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>95</v>
-      </c>
       <c r="F13" s="6" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" ht="42.75" spans="1:15">
@@ -3220,7 +3258,7 @@
         <v>63</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -3238,49 +3276,49 @@
     </row>
     <row r="15" ht="28.5" spans="1:15">
       <c r="A15" s="5" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" ht="42.75" spans="1:15">
@@ -3288,7 +3326,7 @@
         <v>63</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -3306,49 +3344,49 @@
     </row>
     <row r="17" ht="28.5" spans="1:15">
       <c r="A17" s="5" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" ht="42.75" spans="1:15">
@@ -3356,7 +3394,7 @@
         <v>63</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -3374,49 +3412,49 @@
     </row>
     <row r="19" ht="28.5" spans="1:15">
       <c r="A19" s="5" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" ht="42.75" spans="1:15">
@@ -3424,7 +3462,7 @@
         <v>63</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -3461,6 +3499,7 @@
     <hyperlink ref="D8" r:id="rId11" display="Source: Global: Page 3 (&quot;residential customer portfolio... 41.5 million&quot;).&#10;Note: UK figure not separately disclosed in 2024 text; value is estimated based on 2023 figures.&#10;https://www.edf.fr/sites/groupe/files/2025-02/edf-annual-results-2024-management-report-2025-02-21.pdf"/>
     <hyperlink ref="F8" r:id="rId12" display="https://www.edfenergy.com/electric-cars/home-charger"/>
     <hyperlink ref="H8" r:id="rId13" display="Fulfilled by EDF's subsidiary &quot;Contact Solar&quot;. Marketing emphasizes technology types (String vs. Micro inverters) rather than specific manufacturers, allowing for flexible Tier 1 hardware sourcing.&#10;Link: &#10;https://www.contact-solar.co.uk/help-center/our-panels-inverters/" tooltip="https://www.contact-solar.co.uk/help-center/our-panels-inverters/"/>
+    <hyperlink ref="G8" r:id="rId14" display="Adopts a &quot;Hardware Agnostic&quot; strategy: No premium brands (like Tesla Powerwall) are advertised. Focuses on modular, cost-effective solutions installed in-house to maximize margins.&#10;Link: &#10;https://www.contact-solar.co.uk/battery-storage/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
vault backup: 2026-02-03 23:53:26
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="111">
   <si>
     <t>Products/solutions provided</t>
   </si>
@@ -1558,139 +1558,22 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Statkraft (via Mer)</t>
-  </si>
-  <si>
-    <t>NOK ~53.7bn (2022)</t>
-  </si>
-  <si>
-    <t>20+ including UK, DE, NO, SE, AT</t>
-  </si>
-  <si>
-    <t>Broad European</t>
-  </si>
-  <si>
-    <t>Yes (Mer EV charging network)</t>
-  </si>
-  <si>
-    <t>Yes (owns renewable generation)</t>
-  </si>
-  <si>
-    <t>Indirect via partner networks</t>
-  </si>
-  <si>
-    <t>Fleet/Business solutions via Mer</t>
-  </si>
-  <si>
-    <t>Public charging network via Mer</t>
-  </si>
-  <si>
-    <t>Statkraft is Europe’s largest renewable energy producer. (维基百科)</t>
-  </si>
-  <si>
-    <t>Operates EV charging solutions via Mer across multiple European markets. (Mer)</t>
-  </si>
-  <si>
-    <t>Vattenfall AB</t>
-  </si>
-  <si>
-    <t>Large Swedish state‑owned</t>
-  </si>
-  <si>
-    <t>SE, DE, NL, UK</t>
-  </si>
-  <si>
-    <t>Yes (InCharge EV network)</t>
-  </si>
-  <si>
-    <t>Yes (renewables)</t>
-  </si>
-  <si>
-    <t>Yes (workplace fleets)</t>
-  </si>
-  <si>
-    <t>Yes (InCharge public)</t>
-  </si>
-  <si>
-    <t>Vattenfall operates one of Europe’s larger EV networks (InCharge). (Vattenfall)</t>
-  </si>
-  <si>
-    <t>Equinor ASA</t>
-  </si>
-  <si>
-    <t>Large Norwegian energy company</t>
-  </si>
-  <si>
-    <t>30+ countries</t>
-  </si>
-  <si>
-    <t>Very broad</t>
-  </si>
-  <si>
-    <t>Renewable generation &amp; offshore wind</t>
-  </si>
-  <si>
-    <t>Yes (home/business)</t>
-  </si>
-  <si>
-    <t>Yes (commercial)</t>
-  </si>
-  <si>
-    <t>Yes (via partners)</t>
-  </si>
-  <si>
-    <t>Equinor primarily oil/energy with expanding renewables. (维基百科)</t>
-  </si>
-  <si>
-    <t>Iberdrola, S.A.</t>
-  </si>
-  <si>
-    <t>€44.7bn revenue</t>
-  </si>
-  <si>
-    <t>Spain + global footprint</t>
-  </si>
-  <si>
-    <t>~30m customers</t>
-  </si>
-  <si>
-    <t>Yes (charging network deployments in Iberia)</t>
-  </si>
-  <si>
-    <t>Yes (battery projects)</t>
-  </si>
-  <si>
-    <t>Yes (solar &amp; wind)</t>
-  </si>
-  <si>
-    <t>EV tariffs often bundled</t>
-  </si>
-  <si>
-    <t>Major utility with renewables &amp; EV charging expansion in Spain/Portugal. (维基百科)</t>
-  </si>
-  <si>
-    <t>PGE (Polska Grupa Energetyczna)</t>
-  </si>
-  <si>
-    <t>~$16.2bn revenue</t>
-  </si>
-  <si>
-    <t>Poland</t>
-  </si>
-  <si>
-    <t>38m+ Poland</t>
-  </si>
-  <si>
-    <t>Possible EV network partnerships</t>
-  </si>
-  <si>
-    <t>BESS projects planned</t>
-  </si>
-  <si>
-    <t>PV &amp; wind buildout</t>
-  </si>
-  <si>
-    <t>Poland’s largest utility; BESS project planned; India involvement. (维基百科)</t>
+    <t>Fjordkraft</t>
+  </si>
+  <si>
+    <t>Norlys Energi</t>
+  </si>
+  <si>
+    <t>Å Energi / Entelios</t>
+  </si>
+  <si>
+    <t>Vattenfall</t>
+  </si>
+  <si>
+    <t>Statkraft</t>
+  </si>
+  <si>
+    <t>Tibber</t>
   </si>
 </sst>
 </file>
@@ -1703,7 +1586,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1754,6 +1637,14 @@
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -2224,150 +2115,150 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2399,9 +2290,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2730,12 +2625,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>
@@ -2757,11 +2652,11 @@
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="4" t="s">
@@ -2794,7 +2689,7 @@
       <c r="J2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="16" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -2835,7 +2730,7 @@
       <c r="H3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="17" t="s">
         <v>26</v>
       </c>
       <c r="J3" s="7" t="s">
@@ -3090,109 +2985,77 @@
       <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" ht="28.5" spans="1:15">
-      <c r="A11" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>101</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>101</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>101</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>101</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
-    <row r="12" ht="42.75" spans="1:15">
+    <row r="12" spans="1:15">
       <c r="A12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>115</v>
-      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -3206,60 +3069,30 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" ht="15" spans="1:15">
-      <c r="A13" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>122</v>
-      </c>
+    <row r="13" spans="1:15">
+      <c r="A13" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
     </row>
-    <row r="14" ht="42.75" spans="1:15">
+    <row r="14" spans="1:15">
       <c r="A14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>123</v>
-      </c>
+      <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -3274,60 +3107,30 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" ht="28.5" spans="1:15">
-      <c r="A15" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>131</v>
-      </c>
+    <row r="15" spans="1:15">
+      <c r="A15" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
     </row>
-    <row r="16" ht="42.75" spans="1:15">
+    <row r="16" spans="1:15">
       <c r="A16" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>132</v>
-      </c>
+      <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -3342,60 +3145,30 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" ht="28.5" spans="1:15">
-      <c r="A17" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>104</v>
-      </c>
+    <row r="17" spans="1:15">
+      <c r="A17" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
     </row>
-    <row r="18" ht="42.75" spans="1:15">
+    <row r="18" spans="1:15">
       <c r="A18" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>141</v>
-      </c>
+      <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -3410,60 +3183,30 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" ht="28.5" spans="1:15">
-      <c r="A19" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>104</v>
-      </c>
+    <row r="19" spans="1:15">
+      <c r="A19" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
     </row>
-    <row r="20" ht="42.75" spans="1:15">
+    <row r="20" spans="1:15">
       <c r="A20" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>149</v>
-      </c>
+      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -3478,6 +3221,35 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
     </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="E1:I1"/>
@@ -3488,18 +3260,12 @@
     <hyperlink ref="B6" r:id="rId1" display="E.ON Next Drive offers EV‑oriented tariff. (ev.energy)"/>
     <hyperlink ref="F6" r:id="rId2" display="E.ON Next offers Time‑of‑Use Smart Saver tariff. (太阳报)"/>
     <hyperlink ref="B8" r:id="rId3" display="Correction: The PDF screenshot (Page 2, &quot;Sales&quot;) explicitly states 118,690 for 2024.&#10;URL: https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf" tooltip="https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf"/>
-    <hyperlink ref="B12" r:id="rId4" display="Statkraft is Europe’s largest renewable energy producer. (维基百科)"/>
-    <hyperlink ref="C12" r:id="rId5" display="Operates EV charging solutions via Mer across multiple European markets. (Mer)"/>
-    <hyperlink ref="B14" r:id="rId6" display="Vattenfall operates one of Europe’s larger EV networks (InCharge). (Vattenfall)"/>
-    <hyperlink ref="B16" r:id="rId7" display="Equinor primarily oil/energy with expanding renewables. (维基百科)"/>
-    <hyperlink ref="B18" r:id="rId8" display="Major utility with renewables &amp; EV charging expansion in Spain/Portugal. (维基百科)"/>
-    <hyperlink ref="B20" r:id="rId9" display="Poland’s largest utility; BESS project planned; India involvement. (维基百科)"/>
     <hyperlink ref="C8" r:id="rId3" display="Source: Page 32, Note 5.2 text (mentions principal segments: France, UK, Italy).&#10;https://www.edf.fr/sites/groupe/files/2025-03/annual-results-2024-consolidated-financial-statements-2025-03-05.pdf"/>
-    <hyperlink ref="E8" r:id="rId10" display="https://www.edfenergy.com/electric-cars/leasing" tooltip="https://www.edfenergy.com/electric-cars/leasing"/>
-    <hyperlink ref="D8" r:id="rId11" display="Source: Global: Page 3 (&quot;residential customer portfolio... 41.5 million&quot;).&#10;Note: UK figure not separately disclosed in 2024 text; value is estimated based on 2023 figures.&#10;https://www.edf.fr/sites/groupe/files/2025-02/edf-annual-results-2024-management-report-2025-02-21.pdf"/>
-    <hyperlink ref="F8" r:id="rId12" display="https://www.edfenergy.com/electric-cars/home-charger"/>
-    <hyperlink ref="H8" r:id="rId13" display="Fulfilled by EDF's subsidiary &quot;Contact Solar&quot;. Marketing emphasizes technology types (String vs. Micro inverters) rather than specific manufacturers, allowing for flexible Tier 1 hardware sourcing.&#10;Link: &#10;https://www.contact-solar.co.uk/help-center/our-panels-inverters/" tooltip="https://www.contact-solar.co.uk/help-center/our-panels-inverters/"/>
-    <hyperlink ref="G8" r:id="rId14" display="Adopts a &quot;Hardware Agnostic&quot; strategy: No premium brands (like Tesla Powerwall) are advertised. Focuses on modular, cost-effective solutions installed in-house to maximize margins.&#10;Link: &#10;https://www.contact-solar.co.uk/battery-storage/"/>
+    <hyperlink ref="E8" r:id="rId4" display="https://www.edfenergy.com/electric-cars/leasing" tooltip="https://www.edfenergy.com/electric-cars/leasing"/>
+    <hyperlink ref="D8" r:id="rId5" display="Source: Global: Page 3 (&quot;residential customer portfolio... 41.5 million&quot;).&#10;Note: UK figure not separately disclosed in 2024 text; value is estimated based on 2023 figures.&#10;https://www.edf.fr/sites/groupe/files/2025-02/edf-annual-results-2024-management-report-2025-02-21.pdf"/>
+    <hyperlink ref="F8" r:id="rId6" display="https://www.edfenergy.com/electric-cars/home-charger"/>
+    <hyperlink ref="H8" r:id="rId7" display="Fulfilled by EDF's subsidiary &quot;Contact Solar&quot;. Marketing emphasizes technology types (String vs. Micro inverters) rather than specific manufacturers, allowing for flexible Tier 1 hardware sourcing.&#10;Link: &#10;https://www.contact-solar.co.uk/help-center/our-panels-inverters/" tooltip="https://www.contact-solar.co.uk/help-center/our-panels-inverters/"/>
+    <hyperlink ref="G8" r:id="rId8" display="Adopts a &quot;Hardware Agnostic&quot; strategy: No premium brands (like Tesla Powerwall) are advertised. Focuses on modular, cost-effective solutions installed in-house to maximize margins.&#10;Link: &#10;https://www.contact-solar.co.uk/battery-storage/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
vault backup: 2026-02-04 00:44:43
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -2628,9 +2628,9 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
vault backup: 2026-02-04 01:38:48
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="113">
   <si>
     <t>Products/solutions provided</t>
   </si>
@@ -1324,6 +1324,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
       <t>€118.7 Billion</t>
     </r>
     <r>
@@ -1358,6 +1365,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">France (HQ), </t>
     </r>
     <r>
@@ -1383,6 +1396,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">41.5 Million </t>
     </r>
     <r>
@@ -1417,6 +1437,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Partnership with </t>
     </r>
     <r>
@@ -1532,6 +1558,13 @@
   </si>
   <si>
     <t>SottishPower</t>
+  </si>
+  <si>
+    <t>£6.6 Billion (Scottish Power UK plc Total External Revenue for FY ending Dec 2024; -30% YoY decline vs 2023)</t>
+  </si>
+  <si>
+    <t>Source: SPUK_2024_Annual_Accounts.pdf, Page 68 (Consolidated Income Statement).
+https://www.scottishpower.com/userfiles/file/SPUK_2024_Annual_Accounts.pdf</t>
   </si>
   <si>
     <t>SSE plc (UK)</t>
@@ -1586,7 +1619,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1657,13 +1690,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2115,146 +2141,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2630,7 +2656,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>
@@ -2965,11 +2991,13 @@
       </c>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" ht="57" spans="1:15">
       <c r="A9" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -2984,11 +3012,13 @@
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" ht="99.75" spans="1:15">
       <c r="A10" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -3005,49 +3035,49 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="L11" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="M11" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -3071,7 +3101,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="13" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -3109,7 +3139,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="13" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="6"/>
@@ -3147,7 +3177,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="6"/>
@@ -3185,7 +3215,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="13" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="6"/>
@@ -3223,7 +3253,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="13" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="6"/>
@@ -3247,7 +3277,7 @@
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3266,6 +3296,7 @@
     <hyperlink ref="F8" r:id="rId6" display="https://www.edfenergy.com/electric-cars/home-charger"/>
     <hyperlink ref="H8" r:id="rId7" display="Fulfilled by EDF's subsidiary &quot;Contact Solar&quot;. Marketing emphasizes technology types (String vs. Micro inverters) rather than specific manufacturers, allowing for flexible Tier 1 hardware sourcing.&#10;Link: &#10;https://www.contact-solar.co.uk/help-center/our-panels-inverters/" tooltip="https://www.contact-solar.co.uk/help-center/our-panels-inverters/"/>
     <hyperlink ref="G8" r:id="rId8" display="Adopts a &quot;Hardware Agnostic&quot; strategy: No premium brands (like Tesla Powerwall) are advertised. Focuses on modular, cost-effective solutions installed in-house to maximize margins.&#10;Link: &#10;https://www.contact-solar.co.uk/battery-storage/"/>
+    <hyperlink ref="B10" r:id="rId9" display="Source: SPUK_2024_Annual_Accounts.pdf, Page 68 (Consolidated Income Statement).&#10;https://www.scottishpower.com/userfiles/file/SPUK_2024_Annual_Accounts.pdf"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
vault backup: 2026-02-04 02:18:26
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="125">
   <si>
     <t>Products/solutions provided</t>
   </si>
@@ -1563,8 +1563,47 @@
     <t>£6.6 Billion (Scottish Power UK plc Total External Revenue for FY ending Dec 2024; -30% YoY decline vs 2023)</t>
   </si>
   <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>~4.6 Million customers in the UK (Residential &amp; Small Business)</t>
+  </si>
+  <si>
+    <t>Focus on Chargers &amp; Tariffs (No direct leasing)</t>
+  </si>
+  <si>
+    <t>Residential: Wallbox &amp; Indra (Installation via ChargedEV / Plug Me In) Public: ScottishPower Recharge Network (Acquiring ChargePlace Scotland operations in 2026)</t>
+  </si>
+  <si>
+    <t>Primary: Fox ESS (Modular High Voltage); Secondary: Pylontech. Sold mainly as a bundle with Solar PV (not standalone).</t>
+  </si>
+  <si>
+    <t>Primary: JA Solar &amp; Longi (Tier 1 Mono Panels); Inverters: Solis &amp; SolarEdge. Installation via Activ8 Solar partnership.</t>
+  </si>
+  <si>
     <t>Source: SPUK_2024_Annual_Accounts.pdf, Page 68 (Consolidated Income Statement).
 https://www.scottishpower.com/userfiles/file/SPUK_2024_Annual_Accounts.pdf</t>
+  </si>
+  <si>
+    <t>Primary Source: SPUK_2024_Annual_Accounts.pdf, Page 89 (Note 4) - explicitly states operations are within the UK.
+Secondary Source: Official website footer (https://www.scottishpower.co.uk/) confirms registered office in Glasgow, UK.</t>
+  </si>
+  <si>
+    <t>Source: ScottishPower Strategic Report 2023/24. Represents domestic and business customer accounts. (Parent company Iberdrola serves ~100M people globally, but ScottishPower entity is ~4.6M).</t>
+  </si>
+  <si>
+    <t>Strategy differs from Octopus. ScottishPower focuses on selling EV Chargers (e.g., Wallbox Pulsar Max) and offering specialized EV Tariffs for cheaper overnight charging.</t>
+  </si>
+  <si>
+    <t>Differentiation: ScottishPower focuses on direct hardware retail via select partners (Wallbox &amp; Indra), whereas Octopus prioritizes software integration (Kraken) compatible with a wide open ecosystem. Public: SP differentiates as an Owner-Operator (Recharge network + ChargePlace Scotland), unlike pure aggregators.</t>
+  </si>
+  <si>
+    <t>"Solar-led" strategy: Batteries sold only with PV to increase self-consumption. No standalone smart tariff (like Flux) available. Hardware is white-labeled or partnered (Fox ESS) rather than integrated into a proprietary platform like Kraken.
+https://www.scottishpower.co.uk/solar-battery</t>
+  </si>
+  <si>
+    <t>Delivery: Outsourced via Activ8 Solar (vs. Octopus in-house). Tech: Tier 1 Panels (JA Solar/Longi) + Solis/SolarEdge inverters. Warranty: Standard 25-year performance.
+https://api.scottishpower.co.uk/cms-next/files/Solar/Solar_Battery_Heat_Pump_Solution_And_Related_Services_Aug24.pdf</t>
   </si>
   <si>
     <t>SSE plc (UK)</t>
@@ -2654,9 +2693,9 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>
@@ -2991,19 +3030,31 @@
       </c>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" ht="57" spans="1:15">
+    <row r="9" ht="99.75" spans="1:15">
       <c r="A9" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -3012,19 +3063,31 @@
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" ht="99.75" spans="1:15">
+    <row r="10" ht="171" spans="1:15">
       <c r="A10" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+        <v>104</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>110</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -3035,49 +3098,49 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="5" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -3101,7 +3164,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="13" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -3139,7 +3202,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="13" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="6"/>
@@ -3177,7 +3240,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="13" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="6"/>
@@ -3215,7 +3278,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="13" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="6"/>
@@ -3253,7 +3316,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="13" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="6"/>
@@ -3277,7 +3340,7 @@
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="14" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3297,6 +3360,8 @@
     <hyperlink ref="H8" r:id="rId7" display="Fulfilled by EDF's subsidiary &quot;Contact Solar&quot;. Marketing emphasizes technology types (String vs. Micro inverters) rather than specific manufacturers, allowing for flexible Tier 1 hardware sourcing.&#10;Link: &#10;https://www.contact-solar.co.uk/help-center/our-panels-inverters/" tooltip="https://www.contact-solar.co.uk/help-center/our-panels-inverters/"/>
     <hyperlink ref="G8" r:id="rId8" display="Adopts a &quot;Hardware Agnostic&quot; strategy: No premium brands (like Tesla Powerwall) are advertised. Focuses on modular, cost-effective solutions installed in-house to maximize margins.&#10;Link: &#10;https://www.contact-solar.co.uk/battery-storage/"/>
     <hyperlink ref="B10" r:id="rId9" display="Source: SPUK_2024_Annual_Accounts.pdf, Page 68 (Consolidated Income Statement).&#10;https://www.scottishpower.com/userfiles/file/SPUK_2024_Annual_Accounts.pdf"/>
+    <hyperlink ref="G10" r:id="rId10" display="&quot;Solar-led&quot; strategy: Batteries sold only with PV to increase self-consumption. No standalone smart tariff (like Flux) available. Hardware is white-labeled or partnered (Fox ESS) rather than integrated into a proprietary platform like Kraken.&#10;https://www.scottishpower.co.uk/solar-battery"/>
+    <hyperlink ref="H10" r:id="rId11" display="Delivery: Outsourced via Activ8 Solar (vs. Octopus in-house). Tech: Tier 1 Panels (JA Solar/Longi) + Solis/SolarEdge inverters. Warranty: Standard 25-year performance.&#10;https://api.scottishpower.co.uk/cms-next/files/Solar/Solar_Battery_Heat_Pump_Solution_And_Related_Services_Aug24.pdf"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
vault backup: 2026-02-04 04:27:55
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="159">
   <si>
     <t>Products/solutions provided</t>
   </si>
@@ -1578,7 +1578,28 @@
     <t>Primary: Fox ESS (Modular High Voltage); Secondary: Pylontech. Sold mainly as a bundle with Solar PV (not standalone).</t>
   </si>
   <si>
-    <t>Primary: JA Solar &amp; Longi (Tier 1 Mono Panels); Inverters: Solis &amp; SolarEdge. Installation via Activ8 Solar partnership.</t>
+    <t>Tier 1 Monocrystalline Panels (All-black). Inverters: Solis or SolarEdge. Specific brands not guaranteed in marketing materials (White-label strategy).</t>
+  </si>
+  <si>
+    <t>Mitsubishi Electric Ecodan (Air Source). Installation via partner Warmworks or approved network.</t>
+  </si>
+  <si>
+    <t>EV Saver: 7.2p/kWh (12am-5am). Heat Pump Saver: 15p/kWh (11am-4pm). Also offers "Power Saver" events (e.g. Half-price weekends).</t>
+  </si>
+  <si>
+    <t>EV Saver (EVs): 7.2p/kWh fixed overnight rate (12am-5am). Heat Pump Saver (Heating): 15p/kWh daytime rate (11am-4pm). Power Saver (Grid): Ad-hoc "Half-Price Weekend" events.</t>
+  </si>
+  <si>
+    <t>None (Commercial trials only). Currently focuses on V1G (Smart Charging) via EV Saver.</t>
+  </si>
+  <si>
+    <t>~4.6 Million Customers (Big 6). 100% Green Generation (First integrated utility to ditch fossil fuels).</t>
+  </si>
+  <si>
+    <t>Fleet Zero (Leasing via Fleet Alliance). Workplace Charging (Smart Solutions). 100% Green Business Supply (PPAs).</t>
+  </si>
+  <si>
+    <t>ScottishPower Recharge (Rapid/Ultra-rapid Owner-Operator). Key expansion: Taking over "ChargePlace Scotland" operations (Highlands &amp; Islands) in 2026. Destination: Partnership with St Austell Brewery (300+ chargers).</t>
   </si>
   <si>
     <t>Source: SPUK_2024_Annual_Accounts.pdf, Page 68 (Consolidated Income Statement).
@@ -1606,28 +1627,110 @@
 https://api.scottishpower.co.uk/cms-next/files/Solar/Solar_Battery_Heat_Pump_Solution_And_Related_Services_Aug24.pdf</t>
   </si>
   <si>
+    <t>Exclusive Mitsubishi Electric partner. Offers specific "Heat Pump Saver" tariff (15p/kWh) to lower running costs. Installation managed via Warmworks network.
+https://www.scottishpower.com/news/pages/panasonic_partners_to_deliver_greener_warmer_homes_at_lower_cost_for_gb_homeowners.aspx</t>
+  </si>
+  <si>
+    <t>https://www.scottishpower.com/news/pages/scottishpower_launches_its_first_heat_pump_tariff.aspx</t>
+  </si>
+  <si>
+    <t>Differentiation: Unlike Octopus's dynamic ecosystem, SP uses static fixed windows. Key USP: The 11am-4pm Heat Pump window is unique, targeting midday solar generation rather than overnight grid lows. Requirements: Smart Meter (SMETS2) &amp; Direct Debit required.</t>
+  </si>
+  <si>
+    <t>No commercial V2G offer (unlike Octopus Power Pack). Focuses solely on V1G smart charging (EV Saver) after concluding earlier pilot projects.</t>
+  </si>
+  <si>
+    <t>https://www.ofgem.gov.uk/news-and-insight/data/data-portal/retail-market-indicators</t>
+  </si>
+  <si>
+    <t>"Fleet Zero" solution partners with Fleet Alliance for vehicle leasing &amp; management. Offers Workplace Charging installations and Corporate PPAs (direct wind farm supply) for offices.</t>
+  </si>
+  <si>
+    <t>https://www.electrive.com/2025/10/09/scottishpower-to-take-over-ev-charging-in-highlands-and-islands/</t>
+  </si>
+  <si>
     <t>SSE plc (UK)</t>
   </si>
   <si>
-    <t>Major UK supplier</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>Millions</t>
-  </si>
-  <si>
-    <t>—</t>
-  </si>
-  <si>
-    <t>Standard &amp; evolving TOU</t>
-  </si>
-  <si>
-    <t>Standard segments</t>
-  </si>
-  <si>
-    <t>Yes</t>
+    <t>£10.1 bn (FY2025) (Reported Revenue for year ended 31 March 2025)</t>
+  </si>
+  <si>
+    <t>UK &amp; Ireland (Core Utility Markets). Expansion: Spain, France, Italy, Greece, Netherlands, Japan (Renewables only).</t>
+  </si>
+  <si>
+    <t>Network (UK): Distributes to 3.9m homes/businesses (North Scotland &amp; Central Southern England). Retail (Ireland): All-Island market (~7m population). Retail (UK): National coverage (Business Only).</t>
+  </si>
+  <si>
+    <t>None (Infrastructure Focus). Strategy: Provides "Infrastructure-as-a-Service" (Charging) rather than vehicle leasing.</t>
+  </si>
+  <si>
+    <t>UK Domestic: None (Market exited to OVO). Ireland Domestic: Ohme &amp; myenergi (Zappi). UK Commercial: Hardware Agnostic (e.g. Kempower/ABB for depots).</t>
+  </si>
+  <si>
+    <t>Grid-Scale (UK): Major Developer (e.g. Fiddler's Ferry 150MW, Monk Fryston 320MW). Domestic (Ireland): Tesla Powerwall &amp; Solis (via Activ8 JV).</t>
+  </si>
+  <si>
+    <t>UK Domestic: None (Market exited). Ireland: Activ8 Solar Energies (JV). Uses Tier 1 Panels (e.g. Longi/JA). UK Grid-Scale: Major Developer (e.g. Littleton Solar Farm).</t>
+  </si>
+  <si>
+    <t>UK Domestic: None (Market exited to OVO). Ireland: Air-to-Water (Mitsubishi/Daikin via "One Stop Shop"). UK Commercial: District Heating Networks (e.g. Slough, Nathan Road).</t>
+  </si>
+  <si>
+    <t>UK Domestic: None (Retail exited to OVO). Ireland Domestic: Smart Saver Tariffs (Day / Night / Peak). Note: SSE sold its GB domestic business to OVO in 2020. Smart tariffs are only available via SSE Airtricity in Ireland.</t>
+  </si>
+  <si>
+    <t>UK: None (Domestic business sold to OVO). Ireland: Smart Saver (Day / Night / Peak 5-7pm). Ireland Promo: "Saturday Plus" (Free electricity Sat 9am-5pm).</t>
+  </si>
+  <si>
+    <t>—None (Infrastructure trials only). Project: "Bus2Grid" (World's largest V2G trial for London Buses).</t>
+  </si>
+  <si>
+    <t>UK (GB): None (Sold to OVO Energy in 2020). Ireland: ~0.7 Million customers (SSE Airtricity). Generation: 100% Renewable electricity provider (Ireland).</t>
+  </si>
+  <si>
+    <t>Office: Corporate PPAs ("Named Asset" &amp; "Portfolio" options). Fleet Tariff: "SSE Green EV" (100% REGO-backed + Off-peak rates). Infra: Workplace Charging (Design, Build &amp; Operate).</t>
+  </si>
+  <si>
+    <t>SSE Energy Solutions (Ultra-rapid Hubs). Retail Partner: M7 Real Estate (20 locations). Ireland: Partnership with ePower (Forecourts &amp; Hotels).</t>
+  </si>
+  <si>
+    <t>https://www.sse.com/investors/reports-and-results/?year=2025/26</t>
+  </si>
+  <si>
+    <t>https://www.sserenewables.com/international-locations/</t>
+  </si>
+  <si>
+    <t>https://www.ssen.co.uk/about-ssen/who-we-are/</t>
+  </si>
+  <si>
+    <t>https://www.sseenergysolutions.co.uk/business-energy/electric-vehicles</t>
+  </si>
+  <si>
+    <t>https://www.sseairtricity.com/ie/home/home-upgrade/electric-vehicle-charger-installation</t>
+  </si>
+  <si>
+    <t>https://www.sserenewables.com/solar-and-battery/battery-storage/monk-fryston/</t>
+  </si>
+  <si>
+    <t>https://www.sserenewables.com/solar-and-battery/</t>
+  </si>
+  <si>
+    <t>https://www.sseenergysolutions.co.uk/file/partnerships-solutions-brochure</t>
+  </si>
+  <si>
+    <t>https://www.bbc.com/news/business-49310574</t>
+  </si>
+  <si>
+    <t>https://www.bbc.com/news/business-49686218</t>
+  </si>
+  <si>
+    <t>No commercial V2G tariffs. Domestic retail sold to OVO. SSE focuses on custom infrastructure trials like the "Bus2Grid" project (London bus depots).</t>
+  </si>
+  <si>
+    <t>Exited GB domestic market in 2020 (sold customer base to OVO). Now only supplies homes in Ireland (SSE Airtricity, ~0.7m customers). UK focus shifted to Networks &amp; Generation.</t>
+  </si>
+  <si>
+    <t>https://www.sseenergysolutions.co.uk/news-and-insights/ultra-rapid-electric-vehicle-charging-hubs-m7</t>
   </si>
   <si>
     <t>Fjordkraft</t>
@@ -2695,7 +2798,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>
@@ -3030,7 +3133,7 @@
       </c>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" ht="99.75" spans="1:15">
+    <row r="9" ht="128.25" spans="1:15">
       <c r="A9" s="5" t="s">
         <v>96</v>
       </c>
@@ -3055,116 +3158,170 @@
       <c r="H9" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
+      <c r="I9" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="10" ht="171" spans="1:15">
       <c r="A10" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
+        <v>117</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" ht="114" spans="1:15">
       <c r="A11" s="5" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" ht="99.75" spans="1:15">
       <c r="A12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="B12" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
+      <c r="O12" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="13" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -3202,7 +3359,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="13" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="6"/>
@@ -3240,7 +3397,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="13" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="6"/>
@@ -3278,7 +3435,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="13" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="6"/>
@@ -3316,7 +3473,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="13" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="6"/>
@@ -3340,7 +3497,7 @@
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="14" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3362,6 +3519,21 @@
     <hyperlink ref="B10" r:id="rId9" display="Source: SPUK_2024_Annual_Accounts.pdf, Page 68 (Consolidated Income Statement).&#10;https://www.scottishpower.com/userfiles/file/SPUK_2024_Annual_Accounts.pdf"/>
     <hyperlink ref="G10" r:id="rId10" display="&quot;Solar-led&quot; strategy: Batteries sold only with PV to increase self-consumption. No standalone smart tariff (like Flux) available. Hardware is white-labeled or partnered (Fox ESS) rather than integrated into a proprietary platform like Kraken.&#10;https://www.scottishpower.co.uk/solar-battery"/>
     <hyperlink ref="H10" r:id="rId11" display="Delivery: Outsourced via Activ8 Solar (vs. Octopus in-house). Tech: Tier 1 Panels (JA Solar/Longi) + Solis/SolarEdge inverters. Warranty: Standard 25-year performance.&#10;https://api.scottishpower.co.uk/cms-next/files/Solar/Solar_Battery_Heat_Pump_Solution_And_Related_Services_Aug24.pdf"/>
+    <hyperlink ref="I10" r:id="rId12" display="Exclusive Mitsubishi Electric partner. Offers specific &quot;Heat Pump Saver&quot; tariff (15p/kWh) to lower running costs. Installation managed via Warmworks network.&#10;https://www.scottishpower.com/news/pages/panasonic_partners_to_deliver_greener_warmer_homes_at_lower_cost_for_gb_homeowners.aspx"/>
+    <hyperlink ref="J10" r:id="rId13" display="https://www.scottishpower.com/news/pages/scottishpower_launches_its_first_heat_pump_tariff.aspx"/>
+    <hyperlink ref="M10" r:id="rId14" display="https://www.ofgem.gov.uk/news-and-insight/data/data-portal/retail-market-indicators"/>
+    <hyperlink ref="O10" r:id="rId15" display="https://www.electrive.com/2025/10/09/scottishpower-to-take-over-ev-charging-in-highlands-and-islands/"/>
+    <hyperlink ref="B12" r:id="rId16" display="https://www.sse.com/investors/reports-and-results/?year=2025/26"/>
+    <hyperlink ref="C12" r:id="rId17" display="https://www.sserenewables.com/international-locations/"/>
+    <hyperlink ref="D12" r:id="rId18" display="https://www.ssen.co.uk/about-ssen/who-we-are/"/>
+    <hyperlink ref="E12" r:id="rId19" display="https://www.sseenergysolutions.co.uk/business-energy/electric-vehicles"/>
+    <hyperlink ref="F12" r:id="rId20" display="https://www.sseairtricity.com/ie/home/home-upgrade/electric-vehicle-charger-installation"/>
+    <hyperlink ref="G12" r:id="rId21" display="https://www.sserenewables.com/solar-and-battery/battery-storage/monk-fryston/"/>
+    <hyperlink ref="H12" r:id="rId22" display="https://www.sserenewables.com/solar-and-battery/"/>
+    <hyperlink ref="I12" r:id="rId23" display="https://www.sseenergysolutions.co.uk/file/partnerships-solutions-brochure"/>
+    <hyperlink ref="J12" r:id="rId24" display="https://www.bbc.com/news/business-49310574"/>
+    <hyperlink ref="K12" r:id="rId25" display="https://www.bbc.com/news/business-49686218"/>
+    <hyperlink ref="O12" r:id="rId26" display="https://www.sseenergysolutions.co.uk/news-and-insights/ultra-rapid-electric-vehicle-charging-hubs-m7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
vault backup: 2026-02-04 05:11:10
</commit_message>
<xml_diff>
--- a/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
+++ b/Work/二姐/英国及国际能源供应商竞品分析或市场调研数据/Energy supplier data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="187">
   <si>
     <t>Products/solutions provided</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>Public (incl distination, retail etc)</t>
+  </si>
+  <si>
+    <t>Pricing reference</t>
+  </si>
+  <si>
+    <t>Flexibility layer</t>
+  </si>
+  <si>
+    <t>Vehicle-to-grid pilots</t>
   </si>
   <si>
     <t>Octopus Energy Group (Retail) &amp; Kraken Technologies (Software)</t>
@@ -1734,6 +1743,81 @@
   </si>
   <si>
     <t>Fjordkraft</t>
+  </si>
+  <si>
+    <t>NOK 12.2bn (~£0.9bn) (2024 Full Year). Parent: Elmera Group ASA. Trend: Down from NOK 18.9bn in 2023 (due to lower energy prices).</t>
+  </si>
+  <si>
+    <t>Norway (Primary Market, ~30% share). Sweden &amp; Finland (via brand "Nordic Green Energy"). Note: Pure Retailer only (No Grid or Generation assets).</t>
+  </si>
+  <si>
+    <t>Total: ~1.12m Deliveries (1.01m Electricity + 111k Mobile). Core Electricity: 905k (Consumer: 667k, Business: 130k, Nordic: 118k). Alliance Partner Customers: ~107k.</t>
+  </si>
+  <si>
+    <t>None (Retailer Focus). Strategy: Focuses on EV charging optimization (Smart Charging App) and hardware sales, not vehicle leasing.</t>
+  </si>
+  <si>
+    <t>Home: Zaptec &amp; Easee (via Fjordkraft Marketplace). Install: Outsourced to local partners (e.g. "Fiks Ferdig" package). Commercial: None (Focus on residential).</t>
+  </si>
+  <si>
+    <t>Grid-Scale: None (Pure Retailer). Domestic: None / Solar Add-on only. Note: Home batteries are rare in Norway (cheap hydro power).</t>
+  </si>
+  <si>
+    <t>Residential: Rooftop Sales (via Marketplace). Grid-Scale: None (Retailer only). Feature: "Solkonto" (Virtual Battery for surplus power).</t>
+  </si>
+  <si>
+    <t>Residential: Retails Air-to-Air heat pumps via "Marketplace" (Fjordkraft Markedsplass). Key Brands: Toshiba (primary), Panasonic, Mitsubishi. USP: "Interest-free installment" (Rentefri nedbetaling) via electricity bill.</t>
+  </si>
+  <si>
+    <t>667k Consumer Deliveries (Norway). Market Share: ~24% (Largest in Norway). Product: Spot Price (hourly) is the standard model.</t>
+  </si>
+  <si>
+    <t>Office: Spot Price + Portfolio Management ("Forvaltning"). Fleet: "Smartlading Bedrift" (Workplace &amp; Home Reimbursement). Hardware: Zaptec Pro / Easee (Sales &amp; Install). Market Position: Largest B2B supplier in Norway (~22% share).</t>
+  </si>
+  <si>
+    <t>None (No owned network). App Feature: "Ladekart" (Map of public chargers via NOBIL database). Strategy: Focuses on Home Smart Charging (Enode partnership), not public roaming.</t>
+  </si>
+  <si>
+    <t>Standard: Spot Price + 5.90 øre/kWh surcharge + 69 NOK/month fee. Product Name: "Strøm til Spotpris" (Default plan). Fixed Price: Not currently offered to new residential customers (B2B only).</t>
+  </si>
+  <si>
+    <t>Tech Stack: Enode API (Partnership). Consumer Interface: Fjordkraft App (Smart Charging &amp; Heating). Type: Implicit Demand Response (Spot Price Optimization). VPP: None (No consumer aggregation for grid balancing services).</t>
+  </si>
+  <si>
+    <t>None (Focus is on V1G / Smart Charging). Current Tech: Enode API for "Smart Lading" (Price optimization only). Note: No bidirectional charging pilots active.</t>
+  </si>
+  <si>
+    <t>https://elmeragroup.no/globalassets/rapporter/annual-report-2024.pdf</t>
+  </si>
+  <si>
+    <t>No vehicle leasing offer. Focuses purely on Smart Charging services (App-based spot price optimization) and selling home chargers via marketplace.</t>
+  </si>
+  <si>
+    <t>Retails Zaptec &amp; Easee chargers via online Marketplace. Offers "Fiks Ferdig" (Turnkey) installation via partners and interest-free payment plans on energy bills.</t>
+  </si>
+  <si>
+    <t>None. Not listed as a growth initiative in 2024 Report. Low market demand in Norway due to historical cheap hydro generation and effective grid buy-back schemes.</t>
+  </si>
+  <si>
+    <t>Part of "New Growth Initiatives" (NGI). Retails rooftop solar via partners. Offers "Solkonto" (Virtual Battery) to bank surplus energy for winter use.</t>
+  </si>
+  <si>
+    <t>Retails Air-to-Air heat pumps (Toshiba, Panasonic) via partners. Key USP is interest-free repayment integrated into the monthly electricity bill.</t>
+  </si>
+  <si>
+    <t>#1 B2B Supplier (~22% share). Key product is "Portfolio Management" (Active Trading). Fleet solution focuses on automatic reimbursement for employees charging work EVs at home.</t>
+  </si>
+  <si>
+    <t>No owned public chargers or roaming payment service. App provides a map (Ladekart) only. Strategy focuses entirely on Home Smart Charging (Enode partnership).</t>
+  </si>
+  <si>
+    <t>https://www.fjordkraft.no/strom/stromavtale/prisliste/</t>
+  </si>
+  <si>
+    <t>https://enode.com/blog/customers/fjordkraft-partners-with-enode</t>
+  </si>
+  <si>
+    <t>None. Strategy focuses on V1G (Smart Charging) via Enode API to optimize against spot prices. No bidirectional pilots found.</t>
   </si>
   <si>
     <t>Norlys Energi</t>
@@ -2426,7 +2510,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2465,6 +2549,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2793,12 +2883,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.2833333333333" defaultRowHeight="14.25"/>
@@ -2826,7 +2916,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="15"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:18">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -2871,170 +2961,179 @@
       </c>
       <c r="O2" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="P2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" ht="169.5" customHeight="1" spans="1:15">
       <c r="A3" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="85.5" spans="1:15">
       <c r="A4" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="57" spans="1:15">
       <c r="A5" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" ht="29.25" spans="1:15">
       <c r="A6" s="8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="10" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
@@ -3043,323 +3142,385 @@
     </row>
     <row r="7" ht="142.5" spans="1:15">
       <c r="A7" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" ht="171" spans="1:15">
       <c r="A8" s="8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="O8" s="6"/>
     </row>
     <row r="9" ht="128.25" spans="1:15">
       <c r="A9" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" ht="171" spans="1:15">
       <c r="A10" s="8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" ht="114" spans="1:15">
       <c r="A11" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" ht="99.75" spans="1:15">
       <c r="A12" s="8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="12" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" ht="128.25" spans="1:18">
       <c r="A13" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+        <v>156</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>164</v>
+      </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
+      <c r="M13" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q13" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>170</v>
+      </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" ht="99.75" spans="1:18">
       <c r="A14" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>176</v>
+      </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
+      <c r="M14" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="P14" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q14" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>181</v>
+      </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:18">
       <c r="A15" s="13" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="6"/>
@@ -3375,10 +3536,12 @@
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:18">
       <c r="A16" s="8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -3394,10 +3557,12 @@
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:18">
       <c r="A17" s="13" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="6"/>
@@ -3413,10 +3578,12 @@
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:18">
       <c r="A18" s="8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -3432,10 +3599,12 @@
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:18">
       <c r="A19" s="13" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="6"/>
@@ -3451,10 +3620,12 @@
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:18">
       <c r="A20" s="8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -3470,10 +3641,12 @@
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:18">
       <c r="A21" s="13" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="6"/>
@@ -3489,16 +3662,30 @@
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:18">
       <c r="A22" s="8" t="s">
-        <v>63</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:18">
       <c r="A23" s="14" t="s">
-        <v>158</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+    </row>
+    <row r="24" spans="17:18">
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+    </row>
+    <row r="25" spans="17:18">
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3534,6 +3721,12 @@
     <hyperlink ref="J12" r:id="rId24" display="https://www.bbc.com/news/business-49310574"/>
     <hyperlink ref="K12" r:id="rId25" display="https://www.bbc.com/news/business-49686218"/>
     <hyperlink ref="O12" r:id="rId26" display="https://www.sseenergysolutions.co.uk/news-and-insights/ultra-rapid-electric-vehicle-charging-hubs-m7"/>
+    <hyperlink ref="B14" r:id="rId27" display="https://elmeragroup.no/globalassets/rapporter/annual-report-2024.pdf" tooltip="https://elmeragroup.no/globalassets/rapporter/annual-report-2024.pdf"/>
+    <hyperlink ref="C14" r:id="rId27" display="https://elmeragroup.no/globalassets/rapporter/annual-report-2024.pdf" tooltip="https://elmeragroup.no/globalassets/rapporter/annual-report-2024.pdf"/>
+    <hyperlink ref="D14" r:id="rId27" display="https://elmeragroup.no/globalassets/rapporter/annual-report-2024.pdf"/>
+    <hyperlink ref="M14" r:id="rId27" display="https://elmeragroup.no/globalassets/rapporter/annual-report-2024.pdf"/>
+    <hyperlink ref="P14" r:id="rId28" display="https://www.fjordkraft.no/strom/stromavtale/prisliste/"/>
+    <hyperlink ref="Q14" r:id="rId29" display="https://enode.com/blog/customers/fjordkraft-partners-with-enode"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>